<commit_message>
Added DataBase Script And ERD Images And Also Done Modifications/Correction to database.xlsx
</commit_message>
<xml_diff>
--- a/Database/formatted_database.xlsx
+++ b/Database/formatted_database.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\CDAC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishor\Desktop\Project\ProjectDocuments\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF742D1-B4F9-4375-9BE3-2A83ADEC8587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06FFA9A-A069-4C2A-9F67-4B548727FDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C69C6F19-703A-431E-B382-4FB7002DF1D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -319,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,18 +349,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4958DD9B-209F-4537-9713-6C226D001849}">
   <dimension ref="B1:AJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -684,1217 +692,1221 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="H1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="N1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="T1" s="1" t="s">
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="T1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Z1" s="1" t="s">
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Z1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
     </row>
     <row r="2" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="H2" s="3" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="N2" s="3" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="N2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="4"/>
-      <c r="T2" s="3" t="s">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="2"/>
+      <c r="T2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="4"/>
-      <c r="Z2" s="3" t="s">
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="2"/>
+      <c r="Z2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="2"/>
     </row>
     <row r="3" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="2"/>
+      <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="4"/>
+      <c r="K3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="N3" s="3" t="s">
+      <c r="L3" s="2"/>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="4" t="s">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="T3" s="3" t="s">
+      <c r="R3" s="5"/>
+      <c r="T3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="3"/>
-      <c r="W3" s="4" t="s">
+      <c r="V3" s="4"/>
+      <c r="W3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="4"/>
-      <c r="Z3" s="3" t="s">
+      <c r="X3" s="5"/>
+      <c r="Z3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="2"/>
     </row>
     <row r="4" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="2"/>
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="4" t="s">
+      <c r="J4" s="4"/>
+      <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="N4" s="3" t="s">
+      <c r="L4" s="2"/>
+      <c r="N4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="4" t="s">
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="4"/>
-      <c r="T4" s="3" t="s">
+      <c r="R4" s="5"/>
+      <c r="T4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="U4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="3"/>
-      <c r="W4" s="4" t="s">
+      <c r="V4" s="4"/>
+      <c r="W4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="4"/>
-      <c r="Z4" s="3" t="s">
+      <c r="X4" s="5"/>
+      <c r="Z4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AA4" s="3"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="4" t="s">
+      <c r="AA4" s="4"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="4"/>
+      <c r="AD4" s="2"/>
     </row>
     <row r="5" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="H5" s="3" t="s">
+      <c r="F5" s="2"/>
+      <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="4" t="s">
+      <c r="J5" s="4"/>
+      <c r="K5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="N5" s="3" t="s">
+      <c r="L5" s="2"/>
+      <c r="N5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="4" t="s">
+      <c r="P5" s="4"/>
+      <c r="Q5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="4"/>
-      <c r="T5" s="3" t="s">
+      <c r="R5" s="2"/>
+      <c r="T5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="U5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="V5" s="3"/>
-      <c r="W5" s="4" t="s">
+      <c r="V5" s="4"/>
+      <c r="W5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X5" s="4"/>
+      <c r="X5" s="2"/>
     </row>
     <row r="6" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="2"/>
+      <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
+      <c r="L6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
     </row>
     <row r="7" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4" t="s">
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="2"/>
+      <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="4" t="s">
+      <c r="J7" s="4"/>
+      <c r="K7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="4"/>
+      <c r="L7" s="2"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="H8" s="3" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="2"/>
+      <c r="H9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="4" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="4"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="4"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="2"/>
+      <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="4"/>
+      <c r="L10" s="2"/>
     </row>
     <row r="11" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="4"/>
+      <c r="E11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="H11" s="3" t="s">
+      <c r="F11" s="2"/>
+      <c r="H11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="4" t="s">
+      <c r="J11" s="4"/>
+      <c r="K11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="4"/>
+      <c r="L11" s="2"/>
     </row>
     <row r="12" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="H12" s="3" t="s">
+      <c r="F12" s="2"/>
+      <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4" t="s">
+      <c r="J12" s="4"/>
+      <c r="K12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="4"/>
+      <c r="L12" s="2"/>
     </row>
     <row r="19" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="H19" s="1" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="H19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="N19" s="1" t="s">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="N19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="T19" s="1" t="s">
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="T19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Z19" s="1" t="s">
+      <c r="U19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Z19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AF19" s="1" t="s">
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AF19" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="AG19" s="1"/>
-      <c r="AH19" s="1"/>
-      <c r="AI19" s="1"/>
-      <c r="AJ19" s="1"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
     </row>
     <row r="20" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="H20" s="3" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="H20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="4"/>
-      <c r="N20" s="3" t="s">
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="N20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" s="4"/>
-      <c r="T20" s="3" t="s">
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="2"/>
+      <c r="T20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X20" s="4"/>
-      <c r="Z20" s="3" t="s">
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X20" s="2"/>
+      <c r="Z20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD20" s="4"/>
-      <c r="AF20" s="3" t="s">
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="2"/>
+      <c r="AF20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AG20" s="3"/>
-      <c r="AH20" s="3"/>
-      <c r="AI20" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ20" s="2"/>
     </row>
     <row r="21" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="H21" s="3" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="H21" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4" t="s">
+      <c r="J21" s="4"/>
+      <c r="K21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="4"/>
-      <c r="N21" s="3" t="s">
+      <c r="L21" s="2"/>
+      <c r="N21" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R21" s="4"/>
-      <c r="T21" s="3" t="s">
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="T21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X21" s="4"/>
-      <c r="Z21" s="3" t="s">
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="2"/>
+      <c r="Z21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AA21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AC21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD21" s="4"/>
-      <c r="AF21" s="3" t="s">
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="2"/>
+      <c r="AF21" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AG21" s="3"/>
-      <c r="AH21" s="3"/>
-      <c r="AI21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ21" s="2"/>
     </row>
     <row r="22" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="N22" s="3" t="s">
+      <c r="F22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="N22" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R22" s="4"/>
-      <c r="T22" s="3" t="s">
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="2"/>
+      <c r="T22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="U22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="W22" s="4" t="s">
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="X22" s="4"/>
-      <c r="Z22" s="3" t="s">
+      <c r="X22" s="2"/>
+      <c r="Z22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AA22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AC22" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD22" s="4"/>
-      <c r="AF22" s="3" t="s">
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
+      <c r="AC22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="2"/>
+      <c r="AF22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AG22" s="3"/>
-      <c r="AH22" s="3"/>
-      <c r="AI22" s="4" t="s">
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AJ22" s="4"/>
+      <c r="AJ22" s="2"/>
     </row>
     <row r="23" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="Z23" s="3" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="Z23" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AA23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AC23" s="4" t="s">
+      <c r="AA23" s="4"/>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AD23" s="4"/>
+      <c r="AD23" s="2"/>
     </row>
     <row r="24" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="Z24" s="3" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="Z24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AA24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AC24" s="4" t="s">
+      <c r="AA24" s="4"/>
+      <c r="AB24" s="4"/>
+      <c r="AC24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AD24" s="4"/>
+      <c r="AD24" s="2"/>
     </row>
     <row r="25" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="4" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="4"/>
+      <c r="F25" s="2"/>
     </row>
     <row r="26" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2"/>
     </row>
     <row r="27" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="4"/>
+      <c r="F28" s="2"/>
     </row>
     <row r="29" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="4" t="s">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="4"/>
+      <c r="F29" s="2"/>
     </row>
     <row r="30" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="4"/>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="4" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="4"/>
+      <c r="F31" s="2"/>
     </row>
     <row r="32" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="4"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="4" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="4"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="4" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="4"/>
+      <c r="F34" s="2"/>
     </row>
     <row r="35" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="4" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="4"/>
+      <c r="F35" s="5"/>
     </row>
     <row r="36" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="4"/>
+      <c r="F36" s="2"/>
     </row>
     <row r="37" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="4" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="4"/>
+      <c r="F37" s="2"/>
     </row>
     <row r="43" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="H43" s="1" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="H43" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
-      <c r="N43" s="1" t="s">
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="N43" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1"/>
-      <c r="R43" s="1"/>
-      <c r="T43" s="1" t="s">
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="T43" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="X43" s="1"/>
-      <c r="Z43" s="1" t="s">
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Z43" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AA43" s="1"/>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="H44" s="3" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="H44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L44" s="4"/>
-      <c r="N44" s="3" t="s">
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L44" s="2"/>
+      <c r="N44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R44" s="4"/>
-      <c r="T44" s="3" t="s">
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+      <c r="Q44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R44" s="2"/>
+      <c r="T44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X44" s="4"/>
-      <c r="Z44" s="3" t="s">
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X44" s="2"/>
+      <c r="Z44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="3"/>
-      <c r="AC44" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD44" s="4"/>
+      <c r="AA44" s="4"/>
+      <c r="AB44" s="4"/>
+      <c r="AC44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD44" s="2"/>
     </row>
     <row r="45" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="4"/>
-      <c r="H45" s="3" t="s">
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="H45" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L45" s="4"/>
-      <c r="N45" s="3" t="s">
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45" s="2"/>
+      <c r="N45" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="R45" s="4"/>
-      <c r="T45" s="3" t="s">
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R45" s="2"/>
+      <c r="T45" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X45" s="4"/>
-      <c r="Z45" s="3" t="s">
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X45" s="2"/>
+      <c r="Z45" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AA45" s="3"/>
-      <c r="AB45" s="3"/>
-      <c r="AC45" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD45" s="4"/>
+      <c r="AA45" s="4"/>
+      <c r="AB45" s="4"/>
+      <c r="AC45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD45" s="2"/>
     </row>
     <row r="46" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="4" t="s">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F46" s="4"/>
-      <c r="H46" s="3" t="s">
+      <c r="F46" s="5"/>
+      <c r="H46" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L46" s="4"/>
-      <c r="N46" s="3" t="s">
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L46" s="2"/>
+      <c r="N46" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="4" t="s">
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="R46" s="4"/>
-      <c r="T46" s="3" t="s">
+      <c r="R46" s="2"/>
+      <c r="T46" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="X46" s="4"/>
-      <c r="Z46" s="3" t="s">
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X46" s="2"/>
+      <c r="Z46" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
-      <c r="AC46" s="4" t="s">
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AD46" s="4"/>
+      <c r="AD46" s="2"/>
     </row>
     <row r="47" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="4" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="4"/>
-      <c r="T47" s="3" t="s">
+      <c r="F47" s="2"/>
+      <c r="T47" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="4" t="s">
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X47" s="4"/>
+      <c r="X47" s="2"/>
     </row>
     <row r="48" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="4"/>
-      <c r="T48" s="3" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="2"/>
+      <c r="T48" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="4" t="s">
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="X48" s="4"/>
+      <c r="X48" s="2"/>
     </row>
     <row r="49" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="2"/>
     </row>
     <row r="50" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="4" t="s">
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="4"/>
+      <c r="F50" s="2"/>
     </row>
     <row r="51" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="4" t="s">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F51" s="4"/>
+      <c r="F51" s="2"/>
     </row>
     <row r="52" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="4" t="s">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F52" s="4"/>
+      <c r="F52" s="5"/>
     </row>
     <row r="53" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4" t="s">
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="4"/>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="4" t="s">
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="4"/>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="4" t="s">
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="4"/>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4" t="s">
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F56" s="4"/>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4" t="s">
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F57" s="4"/>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="4" t="s">
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F58" s="4"/>
+      <c r="F58" s="2"/>
     </row>
     <row r="63" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
     </row>
     <row r="64" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="4" t="s">
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F65" s="4"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="4" t="s">
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F66" s="4"/>
+      <c r="F66" s="2"/>
     </row>
     <row r="70" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C70" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
     </row>
     <row r="71" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F71" s="4"/>
+      <c r="E71" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="2"/>
     </row>
     <row r="72" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D72" s="3" t="s">
+      <c r="C72" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F72" s="4"/>
+      <c r="E72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="2"/>
     </row>
     <row r="73" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D73" s="3" t="s">
+      <c r="C73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="E73" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="F73" s="4"/>
+      <c r="F73" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="226">
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="K44:L44"/>
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="E71:F71"/>
     <mergeCell ref="E72:F72"/>
@@ -1904,7 +1916,17 @@
     <mergeCell ref="E66:F66"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B72:D72"/>
-    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="T46:V46"/>
+    <mergeCell ref="W46:X46"/>
+    <mergeCell ref="Z46:AB46"/>
+    <mergeCell ref="AC46:AD46"/>
+    <mergeCell ref="N43:R43"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="N46:P46"/>
+    <mergeCell ref="Q46:R46"/>
     <mergeCell ref="B63:F63"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="E64:F64"/>
@@ -1924,26 +1946,20 @@
     <mergeCell ref="W45:X45"/>
     <mergeCell ref="Z45:AB45"/>
     <mergeCell ref="AC45:AD45"/>
-    <mergeCell ref="T46:V46"/>
-    <mergeCell ref="W46:X46"/>
-    <mergeCell ref="Z46:AB46"/>
-    <mergeCell ref="AC46:AD46"/>
     <mergeCell ref="T43:X43"/>
     <mergeCell ref="Z43:AD43"/>
     <mergeCell ref="T44:V44"/>
     <mergeCell ref="W44:X44"/>
     <mergeCell ref="Z44:AB44"/>
     <mergeCell ref="AC44:AD44"/>
-    <mergeCell ref="N43:R43"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="N46:P46"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="H45:J45"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="H46:J46"/>
@@ -1988,6 +2004,14 @@
     <mergeCell ref="AI22:AJ22"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
+    <mergeCell ref="Z19:AD19"/>
+    <mergeCell ref="Z20:AB20"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B37:D37"/>
@@ -2000,9 +2024,6 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="T22:V22"/>
     <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Z19:AD19"/>
-    <mergeCell ref="Z20:AB20"/>
-    <mergeCell ref="AC20:AD20"/>
     <mergeCell ref="Z21:AB21"/>
     <mergeCell ref="AC22:AD22"/>
     <mergeCell ref="Z22:AB22"/>
@@ -2011,15 +2032,10 @@
     <mergeCell ref="Q21:R21"/>
     <mergeCell ref="N22:P22"/>
     <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="W20:X20"/>
     <mergeCell ref="T21:V21"/>
     <mergeCell ref="W21:X21"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="E31:F31"/>
@@ -2053,9 +2069,7 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="T4:V4"/>
-    <mergeCell ref="W4:X4"/>
     <mergeCell ref="T5:V5"/>
-    <mergeCell ref="W5:X5"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="N19:R19"/>
     <mergeCell ref="N20:P20"/>
@@ -2064,14 +2078,11 @@
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:X3"/>
     <mergeCell ref="H11:J11"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H12:J12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="H1:L1"/>
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="N2:P2"/>
@@ -2095,7 +2106,6 @@
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="K7:L7"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="K2:L2"/>
@@ -2120,7 +2130,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changes in Database Done
</commit_message>
<xml_diff>
--- a/Database/formatted_database.xlsx
+++ b/Database/formatted_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kishor\Desktop\Project\ProjectDocuments\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06FFA9A-A069-4C2A-9F67-4B548727FDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60A120C-1132-40F3-9C42-7011736A2753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C69C6F19-703A-431E-B382-4FB7002DF1D6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="86">
   <si>
     <t>owner</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>varchar(255)</t>
+  </si>
+  <si>
+    <t>isacavailable</t>
   </si>
 </sst>
 </file>
@@ -349,22 +352,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4958DD9B-209F-4537-9713-6C226D001849}">
   <dimension ref="B1:AJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q68" sqref="Q68"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -734,46 +740,46 @@
         <v>1</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5"/>
       <c r="H2" s="4" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="K2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="5"/>
       <c r="N2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-      <c r="Q2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R2" s="2"/>
+      <c r="Q2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="5"/>
       <c r="T2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X2" s="2"/>
+      <c r="W2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="5"/>
       <c r="Z2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
-      <c r="AC2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="2"/>
+      <c r="AC2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="5"/>
     </row>
     <row r="3" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="1"/>
@@ -781,10 +787,10 @@
         <v>13</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="5"/>
       <c r="H3" s="4" t="s">
         <v>13</v>
       </c>
@@ -792,21 +798,21 @@
         <v>13</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="N3" s="5" t="s">
+      <c r="L3" s="5"/>
+      <c r="N3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="O3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5" t="s">
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R3" s="5"/>
+      <c r="R3" s="6"/>
       <c r="T3" s="4" t="s">
         <v>28</v>
       </c>
@@ -814,19 +820,19 @@
         <v>13</v>
       </c>
       <c r="V3" s="4"/>
-      <c r="W3" s="5" t="s">
+      <c r="W3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="5"/>
+      <c r="X3" s="6"/>
       <c r="Z3" s="4" t="s">
         <v>33</v>
       </c>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
-      <c r="AC3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="2"/>
+      <c r="AC3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="5"/>
     </row>
     <row r="4" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B4" s="1"/>
@@ -834,10 +840,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="5"/>
       <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
@@ -845,21 +851,21 @@
         <v>13</v>
       </c>
       <c r="J4" s="4"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="N4" s="5" t="s">
+      <c r="L4" s="5"/>
+      <c r="N4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="O4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5" t="s">
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R4" s="5"/>
+      <c r="R4" s="6"/>
       <c r="T4" s="4" t="s">
         <v>25</v>
       </c>
@@ -867,19 +873,19 @@
         <v>13</v>
       </c>
       <c r="V4" s="4"/>
-      <c r="W4" s="5" t="s">
+      <c r="W4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="5"/>
+      <c r="X4" s="6"/>
       <c r="Z4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
-      <c r="AC4" s="2" t="s">
+      <c r="AC4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" s="2"/>
+      <c r="AD4" s="5"/>
     </row>
     <row r="5" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B5" s="1"/>
@@ -887,10 +893,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="5"/>
       <c r="H5" s="4" t="s">
         <v>4</v>
       </c>
@@ -898,10 +904,10 @@
         <v>13</v>
       </c>
       <c r="J5" s="4"/>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="5"/>
       <c r="N5" s="4" t="s">
         <v>11</v>
       </c>
@@ -909,10 +915,10 @@
         <v>13</v>
       </c>
       <c r="P5" s="4"/>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R5" s="2"/>
+      <c r="R5" s="5"/>
       <c r="T5" s="4" t="s">
         <v>11</v>
       </c>
@@ -920,10 +926,10 @@
         <v>13</v>
       </c>
       <c r="V5" s="4"/>
-      <c r="W5" s="2" t="s">
+      <c r="W5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="X5" s="2"/>
+      <c r="X5" s="5"/>
     </row>
     <row r="6" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B6" s="1"/>
@@ -931,10 +937,10 @@
         <v>5</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="5"/>
       <c r="H6" s="4" t="s">
         <v>5</v>
       </c>
@@ -942,12 +948,12 @@
         <v>13</v>
       </c>
       <c r="J6" s="4"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="L6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
     </row>
     <row r="7" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B7" s="1"/>
@@ -955,10 +961,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="5"/>
       <c r="H7" s="4" t="s">
         <v>6</v>
       </c>
@@ -966,11 +972,11 @@
         <v>13</v>
       </c>
       <c r="J7" s="4"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="O7" s="6"/>
+      <c r="L7" s="5"/>
+      <c r="O7" s="2"/>
     </row>
     <row r="8" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B8" s="1"/>
@@ -978,10 +984,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="E8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="5"/>
       <c r="H8" s="4" t="s">
         <v>7</v>
       </c>
@@ -989,10 +995,10 @@
         <v>13</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="2"/>
+      <c r="K8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B9" s="1"/>
@@ -1000,10 +1006,10 @@
         <v>8</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="5"/>
       <c r="H9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1011,10 +1017,10 @@
         <v>13</v>
       </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B10" s="1"/>
@@ -1022,10 +1028,10 @@
         <v>9</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="5"/>
       <c r="H10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1033,10 +1039,10 @@
         <v>13</v>
       </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="2"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B11" s="1"/>
@@ -1044,10 +1050,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="5"/>
       <c r="H11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1055,10 +1061,10 @@
         <v>13</v>
       </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B12" s="1"/>
@@ -1066,10 +1072,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="5"/>
       <c r="H12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1077,10 +1083,10 @@
         <v>13</v>
       </c>
       <c r="J12" s="4"/>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="2"/>
+      <c r="L12" s="5"/>
     </row>
     <row r="19" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B19" s="3" t="s">
@@ -1132,55 +1138,55 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="E20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="5"/>
       <c r="H20" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="2"/>
+      <c r="K20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="5"/>
       <c r="N20" s="4" t="s">
         <v>23</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-      <c r="Q20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R20" s="2"/>
+      <c r="Q20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R20" s="5"/>
       <c r="T20" s="4" t="s">
         <v>23</v>
       </c>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="W20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X20" s="2"/>
+      <c r="W20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X20" s="5"/>
       <c r="Z20" s="4" t="s">
         <v>23</v>
       </c>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
-      <c r="AC20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD20" s="2"/>
+      <c r="AC20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD20" s="5"/>
       <c r="AF20" s="4" t="s">
         <v>23</v>
       </c>
       <c r="AG20" s="4"/>
       <c r="AH20" s="4"/>
-      <c r="AI20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ20" s="2"/>
+      <c r="AI20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ20" s="5"/>
     </row>
     <row r="21" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B21" s="4" t="s">
@@ -1188,10 +1194,10 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="E21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="5"/>
       <c r="H21" s="4" t="s">
         <v>3</v>
       </c>
@@ -1199,46 +1205,46 @@
         <v>13</v>
       </c>
       <c r="J21" s="4"/>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="5"/>
       <c r="N21" s="4" t="s">
         <v>44</v>
       </c>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R21" s="2"/>
+      <c r="Q21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R21" s="5"/>
       <c r="T21" s="4" t="s">
         <v>46</v>
       </c>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="W21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X21" s="2"/>
+      <c r="W21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X21" s="5"/>
       <c r="Z21" s="4" t="s">
         <v>50</v>
       </c>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
-      <c r="AC21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD21" s="2"/>
+      <c r="AC21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD21" s="5"/>
       <c r="AF21" s="4" t="s">
         <v>46</v>
       </c>
       <c r="AG21" s="4"/>
       <c r="AH21" s="4"/>
-      <c r="AI21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AJ21" s="2"/>
+      <c r="AI21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ21" s="5"/>
     </row>
     <row r="22" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B22" s="4" t="s">
@@ -1246,48 +1252,48 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+      <c r="F22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
       <c r="N22" s="4" t="s">
         <v>46</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-      <c r="Q22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R22" s="2"/>
+      <c r="Q22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R22" s="5"/>
       <c r="T22" s="4" t="s">
         <v>47</v>
       </c>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-      <c r="W22" s="2" t="s">
+      <c r="W22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="X22" s="2"/>
+      <c r="X22" s="5"/>
       <c r="Z22" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
-      <c r="AC22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD22" s="2"/>
+      <c r="AC22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD22" s="5"/>
       <c r="AF22" s="4" t="s">
         <v>61</v>
       </c>
       <c r="AG22" s="4"/>
       <c r="AH22" s="4"/>
-      <c r="AI22" s="2" t="s">
+      <c r="AI22" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AJ22" s="2"/>
+      <c r="AJ22" s="5"/>
     </row>
     <row r="23" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B23" s="4" t="s">
@@ -1295,21 +1301,21 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
+      <c r="E23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="Z23" s="4" t="s">
         <v>51</v>
       </c>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
-      <c r="AC23" s="2" t="s">
+      <c r="AC23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AD23" s="2"/>
+      <c r="AD23" s="5"/>
     </row>
     <row r="24" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
@@ -1317,21 +1323,21 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="E24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
       <c r="Z24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="2" t="s">
+      <c r="AC24" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AD24" s="2"/>
+      <c r="AD24" s="5"/>
     </row>
     <row r="25" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B25" s="4" t="s">
@@ -1339,10 +1345,10 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F25" s="2"/>
+      <c r="F25" s="5"/>
     </row>
     <row r="26" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B26" s="4" t="s">
@@ -1350,10 +1356,10 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F26" s="2"/>
+      <c r="E26" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="5"/>
     </row>
     <row r="27" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B27" s="4" t="s">
@@ -1361,10 +1367,10 @@
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
-      <c r="E27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="2"/>
+      <c r="E27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" s="5"/>
     </row>
     <row r="28" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B28" s="4" t="s">
@@ -1372,10 +1378,10 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B29" s="4" t="s">
@@ -1383,21 +1389,21 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="5"/>
     </row>
     <row r="30" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B31" s="4" t="s">
@@ -1405,10 +1411,10 @@
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="5"/>
     </row>
     <row r="32" spans="2:36" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B32" s="4" t="s">
@@ -1416,10 +1422,10 @@
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="2"/>
+      <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B33" s="4" t="s">
@@ -1427,10 +1433,10 @@
       </c>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="2"/>
+      <c r="F33" s="5"/>
     </row>
     <row r="34" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B34" s="4" t="s">
@@ -1438,21 +1444,21 @@
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B36" s="4" t="s">
@@ -1460,10 +1466,10 @@
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="5"/>
     </row>
     <row r="37" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B37" s="4" t="s">
@@ -1471,10 +1477,17 @@
       </c>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="2" t="s">
+      <c r="E37" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="5"/>
+    </row>
+    <row r="38" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="B38" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
     </row>
     <row r="43" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B43" s="3" t="s">
@@ -1519,46 +1532,46 @@
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4"/>
-      <c r="E44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F44" s="2"/>
+      <c r="E44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" s="5"/>
       <c r="H44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
-      <c r="K44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L44" s="2"/>
+      <c r="K44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L44" s="5"/>
       <c r="N44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
-      <c r="Q44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R44" s="2"/>
+      <c r="Q44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R44" s="5"/>
       <c r="T44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
-      <c r="W44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X44" s="2"/>
+      <c r="W44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X44" s="5"/>
       <c r="Z44" s="4" t="s">
         <v>23</v>
       </c>
       <c r="AA44" s="4"/>
       <c r="AB44" s="4"/>
-      <c r="AC44" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD44" s="2"/>
+      <c r="AC44" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD44" s="5"/>
     </row>
     <row r="45" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B45" s="4" t="s">
@@ -1566,93 +1579,93 @@
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F45" s="2"/>
+      <c r="E45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="5"/>
       <c r="H45" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
-      <c r="K45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L45" s="2"/>
+      <c r="K45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L45" s="5"/>
       <c r="N45" s="4" t="s">
         <v>71</v>
       </c>
       <c r="O45" s="4"/>
       <c r="P45" s="4"/>
-      <c r="Q45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="R45" s="2"/>
+      <c r="Q45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R45" s="5"/>
       <c r="T45" s="4" t="s">
         <v>50</v>
       </c>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
-      <c r="W45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X45" s="2"/>
+      <c r="W45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X45" s="5"/>
       <c r="Z45" s="4" t="s">
         <v>71</v>
       </c>
       <c r="AA45" s="4"/>
       <c r="AB45" s="4"/>
-      <c r="AC45" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD45" s="2"/>
+      <c r="AC45" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD45" s="5"/>
     </row>
     <row r="46" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5" t="s">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F46" s="5"/>
+      <c r="F46" s="6"/>
       <c r="H46" s="4" t="s">
         <v>71</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
-      <c r="K46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L46" s="2"/>
+      <c r="K46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L46" s="5"/>
       <c r="N46" s="4" t="s">
         <v>47</v>
       </c>
       <c r="O46" s="4"/>
       <c r="P46" s="4"/>
-      <c r="Q46" s="2" t="s">
+      <c r="Q46" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="R46" s="2"/>
+      <c r="R46" s="5"/>
       <c r="T46" s="4" t="s">
         <v>74</v>
       </c>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
-      <c r="W46" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="X46" s="2"/>
+      <c r="W46" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="X46" s="5"/>
       <c r="Z46" s="4" t="s">
         <v>61</v>
       </c>
       <c r="AA46" s="4"/>
       <c r="AB46" s="4"/>
-      <c r="AC46" s="2" t="s">
+      <c r="AC46" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AD46" s="2"/>
+      <c r="AD46" s="5"/>
     </row>
     <row r="47" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B47" s="4" t="s">
@@ -1660,19 +1673,19 @@
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="2"/>
+      <c r="F47" s="5"/>
       <c r="T47" s="4" t="s">
         <v>51</v>
       </c>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
-      <c r="W47" s="2" t="s">
+      <c r="W47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="X47" s="2"/>
+      <c r="X47" s="5"/>
     </row>
     <row r="48" spans="2:30" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B48" s="4" t="s">
@@ -1680,19 +1693,19 @@
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4"/>
-      <c r="E48" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F48" s="2"/>
+      <c r="E48" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="5"/>
       <c r="T48" s="4" t="s">
         <v>52</v>
       </c>
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
-      <c r="W48" s="2" t="s">
+      <c r="W48" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="X48" s="2"/>
+      <c r="X48" s="5"/>
     </row>
     <row r="49" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B49" s="4" t="s">
@@ -1700,10 +1713,10 @@
       </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
-      <c r="E49" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F49" s="2"/>
+      <c r="E49" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" s="5"/>
     </row>
     <row r="50" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B50" s="4" t="s">
@@ -1711,10 +1724,10 @@
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F50" s="2"/>
+      <c r="F50" s="5"/>
     </row>
     <row r="51" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B51" s="4" t="s">
@@ -1722,21 +1735,21 @@
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F51" s="2"/>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5" t="s">
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F52" s="5"/>
+      <c r="F52" s="6"/>
     </row>
     <row r="53" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B53" s="4" t="s">
@@ -1744,10 +1757,10 @@
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
-      <c r="E53" s="2" t="s">
+      <c r="E53" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F53" s="2"/>
+      <c r="F53" s="5"/>
     </row>
     <row r="54" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B54" s="4" t="s">
@@ -1755,10 +1768,10 @@
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B55" s="4" t="s">
@@ -1766,10 +1779,10 @@
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="2"/>
+      <c r="F55" s="5"/>
     </row>
     <row r="56" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B56" s="4" t="s">
@@ -1777,10 +1790,10 @@
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="2" t="s">
+      <c r="E56" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F56" s="2"/>
+      <c r="F56" s="5"/>
     </row>
     <row r="57" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B57" s="4" t="s">
@@ -1788,10 +1801,10 @@
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="2" t="s">
+      <c r="E57" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F57" s="2"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B58" s="4" t="s">
@@ -1799,10 +1812,10 @@
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F58" s="2"/>
+      <c r="F58" s="5"/>
     </row>
     <row r="63" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B63" s="3" t="s">
@@ -1819,10 +1832,10 @@
       </c>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F64" s="2"/>
+      <c r="E64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B65" s="4" t="s">
@@ -1830,10 +1843,10 @@
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
-      <c r="E65" s="2" t="s">
+      <c r="E65" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F65" s="2"/>
+      <c r="F65" s="5"/>
     </row>
     <row r="66" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B66" s="4" t="s">
@@ -1841,10 +1854,10 @@
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F66" s="2"/>
+      <c r="F66" s="5"/>
     </row>
     <row r="70" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B70" s="3" t="s">
@@ -1867,10 +1880,10 @@
       <c r="D71" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F71" s="2"/>
+      <c r="E71" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F71" s="5"/>
     </row>
     <row r="72" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B72" s="4" t="s">
@@ -1882,10 +1895,10 @@
       <c r="D72" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E72" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F72" s="2"/>
+      <c r="E72" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B73" s="4" t="s">
@@ -1897,41 +1910,181 @@
       <c r="D73" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="E73" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="F73" s="2"/>
+      <c r="F73" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="226">
-    <mergeCell ref="H43:L43"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E72:F72"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="T46:V46"/>
-    <mergeCell ref="W46:X46"/>
-    <mergeCell ref="Z46:AB46"/>
-    <mergeCell ref="AC46:AD46"/>
-    <mergeCell ref="N43:R43"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="N45:P45"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="N46:P46"/>
-    <mergeCell ref="Q46:R46"/>
-    <mergeCell ref="B63:F63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:F65"/>
+  <mergeCells count="227">
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="H8:J8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="T4:V4"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="AC24:AD24"/>
+    <mergeCell ref="Z24:AB24"/>
+    <mergeCell ref="AC21:AD21"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="Z21:AB21"/>
+    <mergeCell ref="AC22:AD22"/>
+    <mergeCell ref="Z22:AB22"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AF20:AH20"/>
+    <mergeCell ref="AI20:AJ20"/>
+    <mergeCell ref="AF21:AH21"/>
+    <mergeCell ref="AI21:AJ21"/>
+    <mergeCell ref="AF22:AH22"/>
+    <mergeCell ref="AI22:AJ22"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="Z19:AD19"/>
+    <mergeCell ref="Z20:AB20"/>
+    <mergeCell ref="AC20:AD20"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="T20:V20"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="T47:V47"/>
     <mergeCell ref="W47:X47"/>
     <mergeCell ref="T48:V48"/>
@@ -1956,180 +2109,41 @@
     <mergeCell ref="W5:X5"/>
     <mergeCell ref="T1:X1"/>
     <mergeCell ref="T2:V2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="T3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="T46:V46"/>
+    <mergeCell ref="W46:X46"/>
+    <mergeCell ref="Z46:AB46"/>
+    <mergeCell ref="AC46:AD46"/>
+    <mergeCell ref="N43:R43"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="N45:P45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="N46:P46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="H43:L43"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E72:F72"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:F65"/>
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="E57:F57"/>
     <mergeCell ref="B58:D58"/>
     <mergeCell ref="E58:F58"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="E47:F47"/>
     <mergeCell ref="B48:D48"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="B49:D49"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AF20:AH20"/>
-    <mergeCell ref="AI20:AJ20"/>
-    <mergeCell ref="AF21:AH21"/>
-    <mergeCell ref="AI21:AJ21"/>
-    <mergeCell ref="AF22:AH22"/>
-    <mergeCell ref="AI22:AJ22"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="Z19:AD19"/>
-    <mergeCell ref="Z20:AB20"/>
-    <mergeCell ref="AC20:AD20"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="T20:V20"/>
-    <mergeCell ref="W20:X20"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="Z23:AB23"/>
-    <mergeCell ref="AC24:AD24"/>
-    <mergeCell ref="Z24:AB24"/>
-    <mergeCell ref="AC21:AD21"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="Z21:AB21"/>
-    <mergeCell ref="AC22:AD22"/>
-    <mergeCell ref="Z22:AB22"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="T4:V4"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="Q20:R20"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="N2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="H7:J7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="H8:J8"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>